<commit_message>
Restate Venezuela y Colombia
</commit_message>
<xml_diff>
--- a/Inventario carolina.xlsx
+++ b/Inventario carolina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carit\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEMPUS\Pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87FD62-063B-4F84-B89C-FE91DCD3D531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66A2028-F7C6-4657-AF25-29809F8239CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{A2D2D3D0-CDA1-4777-B1AC-0F6992CC1937}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{A2D2D3D0-CDA1-4777-B1AC-0F6992CC1937}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTARIO VENEZUELA" sheetId="5" r:id="rId1"/>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1B2F2D-91E0-4DCF-8EC5-AF2D7582B10E}">
   <dimension ref="A1:C186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3271,8 +3271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE2FB93-CB6C-4FF0-B3B6-AEC32E3DBE80}">
   <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:C145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>